<commit_message>
Created file for parameter optimization; changes to metadata
</commit_message>
<xml_diff>
--- a/MetaData/dada2_parameters.xlsx
+++ b/MetaData/dada2_parameters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student/Documents/PollardRotation/dada2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student/Documents/PollardRotation/dada2/MetaData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Dataset</t>
   </si>
@@ -102,6 +102,21 @@
   </si>
   <si>
     <t>c1a_1399_d00</t>
+  </si>
+  <si>
+    <t>Confirmed PE</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>should be paired</t>
+  </si>
+  <si>
+    <t>SRR4423081</t>
+  </si>
+  <si>
+    <t>SRR6121931</t>
   </si>
 </sst>
 </file>
@@ -140,12 +155,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -157,22 +178,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -448,19 +479,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C12"/>
+  <dimension ref="A2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -470,30 +502,39 @@
       <c r="C2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -503,8 +544,11 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -514,8 +558,11 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -525,61 +572,125 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
       </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Screened data for ideal parameters; edited install.packages routine
</commit_message>
<xml_diff>
--- a/MetaData/dada2_parameters.xlsx
+++ b/MetaData/dada2_parameters.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Dataset</t>
   </si>
@@ -117,6 +117,33 @@
   </si>
   <si>
     <t>SRR6121931</t>
+  </si>
+  <si>
+    <t>QualityProfile</t>
+  </si>
+  <si>
+    <t>Quality is pretty shitty…</t>
+  </si>
+  <si>
+    <t>F-truncation</t>
+  </si>
+  <si>
+    <t>R-truncation</t>
+  </si>
+  <si>
+    <t>R2 is pretty shitty</t>
+  </si>
+  <si>
+    <t>Not too bad</t>
+  </si>
+  <si>
+    <t>R1 is unusually terrible</t>
+  </si>
+  <si>
+    <t>R1 is good, R2 less so</t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -482,7 +509,7 @@
   <dimension ref="A2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,9 +517,11 @@
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -505,8 +534,17 @@
       <c r="D2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
@@ -520,7 +558,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -534,7 +572,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -547,8 +585,17 @@
       <c r="D5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5">
+        <v>150</v>
+      </c>
+      <c r="G5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -561,52 +608,72 @@
       <c r="D6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6">
+        <v>200</v>
+      </c>
+      <c r="G6">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8">
+        <v>225</v>
+      </c>
+      <c r="G8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -619,8 +686,17 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11">
+        <v>150</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -633,8 +709,17 @@
       <c r="D12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12">
+        <v>150</v>
+      </c>
+      <c r="G12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -647,8 +732,17 @@
       <c r="D13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13">
+        <v>125</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -660,6 +754,15 @@
       </c>
       <c r="D14" t="s">
         <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14">
+        <v>200</v>
+      </c>
+      <c r="G14">
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="6:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
For real this time, parameters established
</commit_message>
<xml_diff>
--- a/MetaData/dada2_parameters.xlsx
+++ b/MetaData/dada2_parameters.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/student/Documents/PollardRotation/dada2/MetaData/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D21C139-D865-EA4A-AD7A-24BB03C77A61}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>Dataset</t>
   </si>
@@ -47,9 +48,6 @@
     <t>SRR4417483</t>
   </si>
   <si>
-    <t>SRR6121940</t>
-  </si>
-  <si>
     <t>SRR6121890</t>
   </si>
   <si>
@@ -62,9 +60,6 @@
     <t>SRR1914841</t>
   </si>
   <si>
-    <t>TexasAM_TNBS</t>
-  </si>
-  <si>
     <t>UCSD_TNBS</t>
   </si>
   <si>
@@ -116,40 +111,43 @@
     <t>SRR4423081</t>
   </si>
   <si>
-    <t>SRR6121931</t>
-  </si>
-  <si>
-    <t>QualityProfile</t>
-  </si>
-  <si>
-    <t>Quality is pretty shitty…</t>
-  </si>
-  <si>
     <t>F-truncation</t>
   </si>
   <si>
     <t>R-truncation</t>
   </si>
   <si>
-    <t>R2 is pretty shitty</t>
-  </si>
-  <si>
-    <t>Not too bad</t>
-  </si>
-  <si>
-    <t>R1 is unusually terrible</t>
-  </si>
-  <si>
-    <t>R1 is good, R2 less so</t>
-  </si>
-  <si>
-    <t>OK</t>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Consistently has a bad read at ~50bp in R read…</t>
+  </si>
+  <si>
+    <t>Reverse reads are basically 100% garbage…</t>
+  </si>
+  <si>
+    <t>Forward reads are garbage</t>
+  </si>
+  <si>
+    <t>bad read at 230bp in reverse read</t>
+  </si>
+  <si>
+    <t>UCSF_DNR</t>
+  </si>
+  <si>
+    <t>actually could probably accept all 500bp, but the first 300 are definitely the best</t>
+  </si>
+  <si>
+    <t>UTA_TNBS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -216,11 +214,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -238,6 +237,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -505,11 +507,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +519,7 @@
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -529,241 +531,261 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>190</v>
+      </c>
+      <c r="F3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>200</v>
+      </c>
+      <c r="F4">
+        <v>150</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>250</v>
+      </c>
+      <c r="F6">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>250</v>
+      </c>
+      <c r="F7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8">
+        <v>250</v>
+      </c>
+      <c r="F8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5">
-        <v>150</v>
-      </c>
-      <c r="G5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6">
-        <v>200</v>
-      </c>
-      <c r="G6">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8">
-        <v>225</v>
-      </c>
-      <c r="G8">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
+      <c r="C9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9">
+        <v>240</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="2"/>
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>230</v>
+      </c>
+      <c r="F10">
+        <v>175</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <v>240</v>
+      </c>
+      <c r="F11">
+        <v>170</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <v>300</v>
+      </c>
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
         <v>36</v>
       </c>
-      <c r="F11">
-        <v>150</v>
-      </c>
-      <c r="G11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12">
-        <v>150</v>
-      </c>
-      <c r="G12">
-        <v>200</v>
-      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>160</v>
       </c>
       <c r="F13">
-        <v>125</v>
-      </c>
-      <c r="G13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14">
-        <v>200</v>
-      </c>
-      <c r="G14">
-        <v>250</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F20" s="1"/>
@@ -789,19 +811,10 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
   </sheetData>
+  <sortState ref="A4:I13">
+    <sortCondition ref="A3"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>